<commit_message>
- Pagination 객체 구현
</commit_message>
<xml_diff>
--- a/vuejpa/API 설계.xlsx
+++ b/vuejpa/API 설계.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\study\vuejpa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E0C5E84-254B-470E-9E12-826F1E974162}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CD5466E-2234-44EC-9170-1E3BE28C59E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-29325" yWindow="780" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -551,7 +551,7 @@
   <dimension ref="B2:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -662,7 +662,7 @@
     <row r="8" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B8" s="7"/>
       <c r="C8" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>14</v>

</xml_diff>